<commit_message>
Adjust energy counter for no current load
</commit_message>
<xml_diff>
--- a/ChargeTransferFunction.xlsx
+++ b/ChargeTransferFunction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Crouzet automation\Crouzet-Soft\User\EV - 0.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD088611-0B6B-47A7-BAAD-06947AE40B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473D5B1F-7400-4816-82FB-2027B5D9B6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="2205" windowWidth="23925" windowHeight="15885" xr2:uid="{0F769D45-9B41-41DC-836B-7A8B2DBD96AB}"/>
+    <workbookView xWindow="1230" yWindow="2355" windowWidth="23925" windowHeight="15885" xr2:uid="{0F769D45-9B41-41DC-836B-7A8B2DBD96AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>watt</t>
-  </si>
-  <si>
-    <t>deciwatt</t>
-  </si>
-  <si>
-    <t>decisec</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,14 +398,8 @@
       <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="D1">
+        <v>32767</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>